<commit_message>
Add duration feature to playlist tool.
</commit_message>
<xml_diff>
--- a/AVTrack360_record/playlists/dummy.xlsx
+++ b/AVTrack360_record/playlists/dummy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
   <si>
     <t>label</t>
   </si>
@@ -36,9 +36,6 @@
     <t>dummy</t>
   </si>
   <si>
-    <t>rift</t>
-  </si>
-  <si>
     <t>vive</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>mp4</t>
+  </si>
+  <si>
+    <t>duration</t>
   </si>
 </sst>
 </file>
@@ -387,18 +387,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F6:F14"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="19.54296875" customWidth="1"/>
+    <col min="1" max="6" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,131 +406,155 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
+      <c r="C8">
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>